<commit_message>
a new attempt at committing
</commit_message>
<xml_diff>
--- a/df_wflow.xlsx
+++ b/df_wflow.xlsx
@@ -398,10 +398,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>-1.00176269401673</v>
+        <v>-0.608236435814144</v>
       </c>
       <c r="C2" t="n">
-        <v>3.50752444718883</v>
+        <v>-1.81872946919787</v>
       </c>
     </row>
     <row r="3">
@@ -409,10 +409,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>-1.01615465315107</v>
+        <v>0.202516267794457</v>
       </c>
       <c r="C3" t="n">
-        <v>-1.52295354373166</v>
+        <v>1.20638425134075</v>
       </c>
     </row>
     <row r="4">
@@ -420,10 +420,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>-0.40311910543042</v>
+        <v>1.29447715192983</v>
       </c>
       <c r="C4" t="n">
-        <v>5.22577178225862</v>
+        <v>4.43505114580974</v>
       </c>
     </row>
     <row r="5">
@@ -431,10 +431,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.408410218063001</v>
+        <v>-0.275869033621741</v>
       </c>
       <c r="C5" t="n">
-        <v>2.41793441867662</v>
+        <v>-0.71456314590315</v>
       </c>
     </row>
     <row r="6">
@@ -442,10 +442,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>1.51791677118226</v>
+        <v>-0.176039326449044</v>
       </c>
       <c r="C6" t="n">
-        <v>-1.89206233685472</v>
+        <v>0.921891106884248</v>
       </c>
     </row>
     <row r="7">
@@ -453,10 +453,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.545597048759035</v>
+        <v>-0.946062823975874</v>
       </c>
       <c r="C7" t="n">
-        <v>2.08165152525859</v>
+        <v>-1.49122835747614</v>
       </c>
     </row>
     <row r="8">
@@ -464,10 +464,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>-0.488182793699075</v>
+        <v>-2.18966187662582</v>
       </c>
       <c r="C8" t="n">
-        <v>0.26306172346934</v>
+        <v>3.28370102827252</v>
       </c>
     </row>
     <row r="9">
@@ -475,10 +475,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.0257851821469864</v>
+        <v>-0.17430788600259</v>
       </c>
       <c r="C9" t="n">
-        <v>3.6143848167625</v>
+        <v>2.53819688998371</v>
       </c>
     </row>
     <row r="10">
@@ -486,10 +486,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.214325197035093</v>
+        <v>-0.29356529269873</v>
       </c>
       <c r="C10" t="n">
-        <v>3.73719427038262</v>
+        <v>3.57240875105334</v>
       </c>
     </row>
     <row r="11">
@@ -497,10 +497,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>-0.513154107203089</v>
+        <v>0.878130621548514</v>
       </c>
       <c r="C11" t="n">
-        <v>0.562965673323551</v>
+        <v>0.228346786173341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add my first analysis
</commit_message>
<xml_diff>
--- a/df_wflow.xlsx
+++ b/df_wflow.xlsx
@@ -398,10 +398,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="n">
-        <v>-0.608236435814144</v>
+        <v>-1.00176269401673</v>
       </c>
       <c r="C2" t="n">
-        <v>-1.81872946919787</v>
+        <v>3.50752444718883</v>
       </c>
     </row>
     <row r="3">
@@ -409,10 +409,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="n">
-        <v>0.202516267794457</v>
+        <v>-1.01615465315107</v>
       </c>
       <c r="C3" t="n">
-        <v>1.20638425134075</v>
+        <v>-1.52295354373166</v>
       </c>
     </row>
     <row r="4">
@@ -420,10 +420,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="n">
-        <v>1.29447715192983</v>
+        <v>-0.40311910543042</v>
       </c>
       <c r="C4" t="n">
-        <v>4.43505114580974</v>
+        <v>5.22577178225862</v>
       </c>
     </row>
     <row r="5">
@@ -431,10 +431,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="n">
-        <v>-0.275869033621741</v>
+        <v>-0.408410218063001</v>
       </c>
       <c r="C5" t="n">
-        <v>-0.71456314590315</v>
+        <v>2.41793441867662</v>
       </c>
     </row>
     <row r="6">
@@ -442,10 +442,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="n">
-        <v>-0.176039326449044</v>
+        <v>1.51791677118226</v>
       </c>
       <c r="C6" t="n">
-        <v>0.921891106884248</v>
+        <v>-1.89206233685472</v>
       </c>
     </row>
     <row r="7">
@@ -453,10 +453,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="n">
-        <v>-0.946062823975874</v>
+        <v>-0.545597048759035</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.49122835747614</v>
+        <v>2.08165152525859</v>
       </c>
     </row>
     <row r="8">
@@ -464,10 +464,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="n">
-        <v>-2.18966187662582</v>
+        <v>-0.488182793699075</v>
       </c>
       <c r="C8" t="n">
-        <v>3.28370102827252</v>
+        <v>0.26306172346934</v>
       </c>
     </row>
     <row r="9">
@@ -475,10 +475,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="n">
-        <v>-0.17430788600259</v>
+        <v>-0.0257851821469864</v>
       </c>
       <c r="C9" t="n">
-        <v>2.53819688998371</v>
+        <v>3.6143848167625</v>
       </c>
     </row>
     <row r="10">
@@ -486,10 +486,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="n">
-        <v>-0.29356529269873</v>
+        <v>-0.214325197035093</v>
       </c>
       <c r="C10" t="n">
-        <v>3.57240875105334</v>
+        <v>3.73719427038262</v>
       </c>
     </row>
     <row r="11">
@@ -497,10 +497,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="n">
-        <v>0.878130621548514</v>
+        <v>-0.513154107203089</v>
       </c>
       <c r="C11" t="n">
-        <v>0.228346786173341</v>
+        <v>0.562965673323551</v>
       </c>
     </row>
   </sheetData>

</xml_diff>